<commit_message>
New message data RM
</commit_message>
<xml_diff>
--- a/rslt.xlsx
+++ b/rslt.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>X1</t>
   </si>
@@ -38,6 +38,9 @@
     <t/>
   </si>
   <si>
+    <t>sexe (m)</t>
+  </si>
+  <si>
     <t>atopie (1)</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
     <t>OR</t>
   </si>
   <si>
+    <t>3.281</t>
+  </si>
+  <si>
     <t>0.75</t>
   </si>
   <si>
@@ -56,6 +62,9 @@
     <t>IC</t>
   </si>
   <si>
+    <t>[0.666;24.445]</t>
+  </si>
+  <si>
     <t>[0.159;3.358]</t>
   </si>
   <si>
@@ -65,10 +74,16 @@
     <t>pval</t>
   </si>
   <si>
+    <t>0.176</t>
+  </si>
+  <si>
     <t>0.705</t>
   </si>
   <si>
     <t>0.092</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>0.926</t>
@@ -165,22 +180,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -188,19 +203,19 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -211,22 +226,45 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
-        <v>24</v>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>